<commit_message>
Update excel spreadsheet with large struct benchmark
</commit_message>
<xml_diff>
--- a/docs/vlm-benchmarks.xlsx
+++ b/docs/vlm-benchmarks.xlsx
@@ -5,17 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhyang/Google Drive (jy2816@columbia.edu)/Columbia/Senior/Spring/C++/vector-list-test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhyang/Google Drive (jy2816@columbia.edu)/Columbia/Senior/Spring/C++/vector-list-test/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273EE6F5-6104-7947-8FD2-7419CE2337F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB010079-93DB-2746-86B5-57AF4EE58730}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="480" windowWidth="28040" windowHeight="16780" xr2:uid="{A1566076-2BF5-424B-9F5A-D6378F2678BB}"/>
+    <workbookView xWindow="-380" yWindow="2540" windowWidth="28040" windowHeight="16700" xr2:uid="{A1566076-2BF5-424B-9F5A-D6378F2678BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$2:$E$9</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$F$2:$F$9</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$G$2:$G$9</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>map</t>
   </si>
@@ -619,7 +628,564 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Vector-List-Map</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Comparison (Large Struct)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vector</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.28963E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4928800000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7418199999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>2.77921E-2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>9.7052899999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4.4761699999999998</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>23.411899999999999</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>948.529</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B4A1-0449-81C9-0AB13EA10B1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>list</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.21203E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3603000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.42557E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0510699999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9709300000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.63072700000000004</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>3.5529299999999999</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>285.24700000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B4A1-0449-81C9-0AB13EA10B1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.4728000000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8021000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5446300000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>2.5410300000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>8.2297700000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.28912700000000002</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.23098</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>88.690399999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B4A1-0449-81C9-0AB13EA10B1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="44737775"/>
+        <c:axId val="44664175"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="44737775"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="44664175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="44664175"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="44737775"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1162,20 +1728,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>185420</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>195579</xdr:rowOff>
+      <xdr:colOff>124460</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>124459</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>402197</xdr:colOff>
+      <xdr:colOff>341237</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>13400</xdr:rowOff>
+      <xdr:rowOff>145480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1195,6 +2264,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>767080</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>40640</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>71120</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E380493D-8B87-E144-88DE-BF92A4D958A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1502,8 +2607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C40599-3A6A-3343-9FC9-31948B8D938E}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1518,8 +2623,15 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1532,8 +2644,15 @@
       <c r="C2" s="1">
         <v>8.3340000000000002E-6</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="E2" s="1">
+        <v>2.28963E-5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.21203E-5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4.4728000000000003E-5</v>
+      </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1546,8 +2665,15 @@
       <c r="C3" s="1">
         <v>4.0667699999999997E-5</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="E3" s="1">
+        <v>2.4928800000000002E-4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5.3603000000000002E-5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.8021000000000001E-4</v>
+      </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1560,9 +2686,15 @@
       <c r="C4" s="1">
         <v>9.4668999999999998E-5</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="1">
+        <v>9.7418199999999998E-4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.42557E-4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3.5446300000000001E-4</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1577,8 +2709,15 @@
       <c r="C5">
         <v>9.3902299999999998E-4</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="E5">
+        <v>2.77921E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.0510699999999999E-3</v>
+      </c>
+      <c r="G5">
+        <v>2.5410300000000001E-3</v>
+      </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1591,8 +2730,15 @@
       <c r="C6">
         <v>3.9394299999999998E-3</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="E6">
+        <v>9.7052899999999998E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>8.9709300000000002E-3</v>
+      </c>
+      <c r="G6">
+        <v>8.2297700000000008E-3</v>
+      </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1605,8 +2751,15 @@
       <c r="C7">
         <v>9.1670199999999993E-2</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7">
+        <v>4.4761699999999998</v>
+      </c>
+      <c r="F7">
+        <v>0.63072700000000004</v>
+      </c>
+      <c r="G7">
+        <v>0.28912700000000002</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1619,8 +2772,15 @@
       <c r="C8">
         <v>0.44479099999999999</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="E8">
+        <v>23.411899999999999</v>
+      </c>
+      <c r="F8">
+        <v>3.5529299999999999</v>
+      </c>
+      <c r="G8">
+        <v>1.23098</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1633,8 +2793,15 @@
       <c r="C9">
         <v>20.9361</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9">
+        <v>948.529</v>
+      </c>
+      <c r="F9">
+        <v>285.24700000000001</v>
+      </c>
+      <c r="G9">
+        <v>88.690399999999997</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1647,8 +2814,6 @@
       <c r="C10">
         <v>203.75700000000001</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>

</xml_diff>

<commit_message>
Move write-up into docs
</commit_message>
<xml_diff>
--- a/docs/vlm-benchmarks.xlsx
+++ b/docs/vlm-benchmarks.xlsx
@@ -8,23 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhyang/Google Drive (jy2816@columbia.edu)/Columbia/Senior/Spring/C++/vector-list-test/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB010079-93DB-2746-86B5-57AF4EE58730}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C46867B-E72C-AA49-A061-B2E8961698DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-380" yWindow="2540" windowWidth="28040" windowHeight="16700" xr2:uid="{A1566076-2BF5-424B-9F5A-D6378F2678BB}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16700" xr2:uid="{A1566076-2BF5-424B-9F5A-D6378F2678BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$2:$E$9</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$F$2:$F$9</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$G$2:$G$9</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
     <t>map</t>
   </si>
@@ -49,13 +40,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,9 +75,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1145,6 +1143,1062 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Vector-List-Map Large Struct Comparison (-O2)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vector</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.3594000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8345699999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5519999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5600899999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0.100826</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4.3540700000000001</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>33.99</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>709.63199999999995</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>26884.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-97C1-4944-88AD-1391650A3C51}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>list</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.9753299999999998E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8292700000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8854699999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>1.7075E-3</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>6.7436500000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.37466100000000002</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>4.74946</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>155.309</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>1896.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-97C1-4944-88AD-1391650A3C51}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>9.4239999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2328700000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7927299999999995E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>6.9641799999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.2699700000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.24557100000000001</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.3441399999999999</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>93.498199999999997</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>588.26900000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-97C1-4944-88AD-1391650A3C51}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1619704016"/>
+        <c:axId val="1620654384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1619704016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1620654384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1620654384"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1619704016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Vector-List-Map Comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (-O2)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vector</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8.9800000000000002E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6286699999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2713300000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0899700000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.4861E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>2.7317299999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.38091E-2</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>0.30247000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>1.99332</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>6.3984500000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA45-9B4E-8455-9B58128A9C82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>list</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.0666699999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6583300000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1194300000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>1.8185599999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>6.7259000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>5.9803200000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.32227899999999998</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>16.372399999999999</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>174.96100000000001</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>1259.4100000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AA45-9B4E-8455-9B58128A9C82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.9766699999999998E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6637300000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0321699999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>4.1046000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.57197E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>7.9239799999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.36235400000000001</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>17.9145</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>163.03899999999999</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>954.66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AA45-9B4E-8455-9B58128A9C82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1656459472"/>
+        <c:axId val="1656084432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1656459472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1656084432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1656084432"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1656459472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1225,6 +2279,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1729,6 +2863,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2271,16 +4411,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>767080</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>148136</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>88356</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>40640</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>71120</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>249464</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>108676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2300,6 +4440,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>552663</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>189894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>737053</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49719281-AD4E-CB4E-B5DB-A09D21BA8F7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>170131</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>96087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>826697</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>131792</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E18623F-8B8D-224A-BF06-89E0436CDDE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2605,15 +4817,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C40599-3A6A-3343-9FC9-31948B8D938E}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2633,8 +4845,30 @@
         <v>0</v>
       </c>
       <c r="H1" s="1"/>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1.1667E-5</v>
       </c>
@@ -2654,8 +4888,31 @@
         <v>4.4728000000000003E-5</v>
       </c>
       <c r="H2" s="1"/>
+      <c r="I2" s="1">
+        <v>8.9800000000000002E-7</v>
+      </c>
+      <c r="J2" s="1">
+        <v>9.0666699999999998E-7</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2.9766699999999998E-6</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1">
+        <v>1.3594000000000001E-5</v>
+      </c>
+      <c r="N2" s="1">
+        <v>5.9753299999999998E-6</v>
+      </c>
+      <c r="O2" s="1">
+        <v>9.4239999999999999E-6</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>4.6668300000000002E-5</v>
       </c>
@@ -2675,8 +4932,30 @@
         <v>1.8021000000000001E-4</v>
       </c>
       <c r="H3" s="1"/>
+      <c r="I3" s="1">
+        <v>2.6286699999999999E-6</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3.6583300000000002E-6</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1.6637300000000001E-5</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1">
+        <v>1.8345699999999999E-4</v>
+      </c>
+      <c r="N3" s="1">
+        <v>2.8292700000000001E-5</v>
+      </c>
+      <c r="O3" s="1">
+        <v>3.2328700000000001E-5</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1.1700400000000001E-4</v>
       </c>
@@ -2696,10 +4975,26 @@
         <v>3.5446300000000001E-4</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="1">
+        <v>5.2713300000000002E-6</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.1194300000000001E-5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4.0321699999999997E-5</v>
+      </c>
+      <c r="M4" s="1">
+        <v>6.5519999999999999E-4</v>
+      </c>
+      <c r="N4" s="1">
+        <v>9.8854699999999994E-5</v>
+      </c>
+      <c r="O4" s="1">
+        <v>7.7927299999999995E-5</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1.40905E-3</v>
       </c>
@@ -2719,8 +5014,26 @@
         <v>2.5410300000000001E-3</v>
       </c>
       <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <v>5.0899700000000003E-5</v>
+      </c>
+      <c r="J5">
+        <v>1.8185599999999999E-4</v>
+      </c>
+      <c r="K5">
+        <v>4.1046000000000002E-4</v>
+      </c>
+      <c r="M5" s="1">
+        <v>2.5600899999999999E-2</v>
+      </c>
+      <c r="N5">
+        <v>1.7075E-3</v>
+      </c>
+      <c r="O5">
+        <v>6.9641799999999997E-4</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6.4292400000000001E-3</v>
       </c>
@@ -2740,8 +5053,26 @@
         <v>8.2297700000000008E-3</v>
       </c>
       <c r="H6" s="1"/>
+      <c r="I6">
+        <v>1.4861E-4</v>
+      </c>
+      <c r="J6">
+        <v>6.7259000000000004E-4</v>
+      </c>
+      <c r="K6">
+        <v>1.57197E-3</v>
+      </c>
+      <c r="M6">
+        <v>0.100826</v>
+      </c>
+      <c r="N6">
+        <v>6.7436500000000003E-3</v>
+      </c>
+      <c r="O6">
+        <v>3.2699700000000001E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.12662000000000001</v>
       </c>
@@ -2761,8 +5092,26 @@
         <v>0.28912700000000002</v>
       </c>
       <c r="H7" s="1"/>
+      <c r="I7">
+        <v>2.7317299999999999E-3</v>
+      </c>
+      <c r="J7">
+        <v>5.9803200000000001E-2</v>
+      </c>
+      <c r="K7">
+        <v>7.9239799999999999E-2</v>
+      </c>
+      <c r="M7">
+        <v>4.3540700000000001</v>
+      </c>
+      <c r="N7">
+        <v>0.37466100000000002</v>
+      </c>
+      <c r="O7">
+        <v>0.24557100000000001</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.43796200000000002</v>
       </c>
@@ -2782,8 +5131,26 @@
         <v>1.23098</v>
       </c>
       <c r="H8" s="1"/>
+      <c r="I8">
+        <v>1.38091E-2</v>
+      </c>
+      <c r="J8">
+        <v>0.32227899999999998</v>
+      </c>
+      <c r="K8">
+        <v>0.36235400000000001</v>
+      </c>
+      <c r="M8">
+        <v>33.99</v>
+      </c>
+      <c r="N8">
+        <v>4.74946</v>
+      </c>
+      <c r="O8">
+        <v>1.3441399999999999</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>10.456799999999999</v>
       </c>
@@ -2803,8 +5170,26 @@
         <v>88.690399999999997</v>
       </c>
       <c r="H9" s="1"/>
+      <c r="I9">
+        <v>0.30247000000000002</v>
+      </c>
+      <c r="J9">
+        <v>16.372399999999999</v>
+      </c>
+      <c r="K9">
+        <v>17.9145</v>
+      </c>
+      <c r="M9">
+        <v>709.63199999999995</v>
+      </c>
+      <c r="N9">
+        <v>155.309</v>
+      </c>
+      <c r="O9">
+        <v>93.498199999999997</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>47.851999999999997</v>
       </c>
@@ -2815,9 +5200,26 @@
         <v>203.75700000000001</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10">
+        <v>1.99332</v>
+      </c>
+      <c r="J10">
+        <v>174.96100000000001</v>
+      </c>
+      <c r="K10">
+        <v>163.03899999999999</v>
+      </c>
+      <c r="M10">
+        <v>26884.1</v>
+      </c>
+      <c r="N10">
+        <v>1896.46</v>
+      </c>
+      <c r="O10">
+        <v>588.26900000000001</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>171.40700000000001</v>
       </c>
@@ -2826,6 +5228,15 @@
       </c>
       <c r="C11">
         <v>1225.1500000000001</v>
+      </c>
+      <c r="I11">
+        <v>6.3984500000000004</v>
+      </c>
+      <c r="J11">
+        <v>1259.4100000000001</v>
+      </c>
+      <c r="K11">
+        <v>954.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>